<commit_message>
Updated By Shiping Ver1.1
</commit_message>
<xml_diff>
--- a/ClusterTraining.xlsx
+++ b/ClusterTraining.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT PROJECTS\Shipin3x\Shipin3x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C3E704-2342-4DE7-9EE8-4DBF92A9031C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA329BF-365F-4991-B849-83C6F136F4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="135">
   <si>
     <t>CurrDate</t>
   </si>
@@ -451,6 +451,9 @@
   <si>
     <t>To config Jenkins files in github</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -464,7 +467,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tw Cen MT"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -472,20 +475,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tw Cen MT"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tw Cen MT"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tw Cen MT"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -512,7 +515,7 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tw Cen MT"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1183,16 +1186,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1213,11 +1222,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1245,33 +1275,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1520,87 +1523,87 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G31" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G31" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G32" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G32" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G33" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G33" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G12" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G12" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$AD$6" max="12" min="1" page="10" val="5"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$AD$6" max="12" min="1" page="10" val="4"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$13" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$13" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$14" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$14" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$15" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$15" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$16" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$16" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$17" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$17" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$18" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$18" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1608,43 +1611,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$19" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$19" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$20" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$20" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$21" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$21" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$23" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$23" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G11" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G11" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G$24" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G$24" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G27" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G27" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G35" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G35" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G36" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G36" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1652,43 +1655,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G37" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G37" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G38" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G38" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp42.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G39" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G39" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp43.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G41" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G41" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp44.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G42" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G42" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G43" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G43" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G46" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G46" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G47" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G47" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G48" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G48" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G49" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G49" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1696,15 +1699,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp50.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G50" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G50" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G51" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G51" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G53" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G53" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp53.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1780,7 +1783,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G26" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G26" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1796,11 +1799,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G29" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G29" lockText="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$G30" lockText="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$G30" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7663,9 +7666,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Droplet">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Droplet">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7673,48 +7676,48 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="355071"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="AABED7"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="2FA3EE"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="4BCAAD"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="86C157"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="D99C3F"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="CE6633"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="A35DD1"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="56BCFE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="97C5E3"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Droplet">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Tw Cen MT" panose="020B0602020104020603"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -7740,16 +7743,16 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Tw Cen MT" panose="020B0602020104020603"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -7775,8 +7778,103 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Droplet">
       <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="69000"/>
+            <a:satMod val="105000"/>
+            <a:lumMod val="110000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="94000"/>
+                <a:satMod val="100000"/>
+                <a:lumMod val="108000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="100000"/>
+                <a:lumMod val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="72000"/>
+                <a:satMod val="120000"/>
+                <a:lumMod val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="25400" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="28000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="63500" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="69000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="balanced" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d prstMaterial="plastic">
+            <a:bevelT w="25400" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -7784,23 +7882,14 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="90000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:shade val="64000"/>
+                <a:lumMod val="88000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -7810,101 +7899,18 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="84000"/>
                 <a:shade val="100000"/>
+                <a:hueMod val="130000"/>
+                <a:satMod val="150000"/>
+                <a:lumMod val="112000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="92000"/>
+                <a:satMod val="140000"/>
+                <a:lumMod val="110000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -7917,7 +7923,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Droplet" id="{8984A317-299A-4E50-B45D-BFC9EDE2337A}" vid="{A633B6A3-9E7F-4C10-9C98-2517A3134361}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7931,24 +7937,24 @@
   <dimension ref="C1:AU22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="5.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="47" width="3.33203125" style="1" customWidth="1"/>
-    <col min="48" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="2.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.796875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="8.69921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.3984375" style="1" customWidth="1"/>
+    <col min="10" max="47" width="3.296875" style="1" customWidth="1"/>
+    <col min="48" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:47" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:47" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="64"/>
       <c r="D1" s="64"/>
       <c r="E1" s="64"/>
@@ -7995,7 +8001,7 @@
       <c r="AT1" s="64"/>
       <c r="AU1" s="64"/>
     </row>
-    <row r="2" spans="3:47" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:47" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="64"/>
       <c r="D2" s="64"/>
       <c r="E2" s="64"/>
@@ -8042,7 +8048,7 @@
       <c r="AT2" s="64"/>
       <c r="AU2" s="64"/>
     </row>
-    <row r="3" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C3" s="65" t="s">
         <v>14</v>
       </c>
@@ -8091,7 +8097,7 @@
       <c r="AT3" s="66"/>
       <c r="AU3" s="67"/>
     </row>
-    <row r="4" spans="3:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:47" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="68"/>
       <c r="D4" s="69"/>
       <c r="E4" s="69"/>
@@ -8138,7 +8144,7 @@
       <c r="AT4" s="69"/>
       <c r="AU4" s="70"/>
     </row>
-    <row r="5" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C5" s="71" t="s">
         <v>0</v>
       </c>
@@ -8194,7 +8200,7 @@
       <c r="AT5" s="5"/>
       <c r="AU5" s="10"/>
     </row>
-    <row r="6" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C6" s="73" t="s">
         <v>18</v>
       </c>
@@ -8231,7 +8237,7 @@
       <c r="AB6" s="78"/>
       <c r="AC6" s="78"/>
       <c r="AD6" s="19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE6" s="5"/>
       <c r="AF6" s="5"/>
@@ -8251,7 +8257,7 @@
       <c r="AT6" s="5"/>
       <c r="AU6" s="10"/>
     </row>
-    <row r="7" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C7" s="25"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -8298,7 +8304,7 @@
       <c r="AT7" s="5"/>
       <c r="AU7" s="10"/>
     </row>
-    <row r="8" spans="3:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="76" t="s">
         <v>13</v>
       </c>
@@ -8435,7 +8441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C9" s="76"/>
       <c r="D9" s="75"/>
       <c r="E9" s="75"/>
@@ -8445,158 +8451,158 @@
       <c r="I9" s="75"/>
       <c r="J9" s="9">
         <f>DATE($V$6,$AD$6,1)-WEEKDAY(DATE($V$6,$AD$6,1),1)+1</f>
-        <v>44682</v>
+        <v>44647</v>
       </c>
       <c r="K9" s="9">
         <f>J9+1</f>
-        <v>44683</v>
+        <v>44648</v>
       </c>
       <c r="L9" s="9">
         <f t="shared" ref="L9:AU9" si="0">K9+1</f>
-        <v>44684</v>
+        <v>44649</v>
       </c>
       <c r="M9" s="9">
         <f t="shared" si="0"/>
-        <v>44685</v>
+        <v>44650</v>
       </c>
       <c r="N9" s="9">
         <f t="shared" si="0"/>
-        <v>44686</v>
+        <v>44651</v>
       </c>
       <c r="O9" s="9">
         <f t="shared" si="0"/>
-        <v>44687</v>
+        <v>44652</v>
       </c>
       <c r="P9" s="9">
         <f t="shared" si="0"/>
-        <v>44688</v>
+        <v>44653</v>
       </c>
       <c r="Q9" s="9">
         <f t="shared" si="0"/>
-        <v>44689</v>
+        <v>44654</v>
       </c>
       <c r="R9" s="9">
         <f t="shared" si="0"/>
-        <v>44690</v>
+        <v>44655</v>
       </c>
       <c r="S9" s="9">
         <f t="shared" si="0"/>
-        <v>44691</v>
+        <v>44656</v>
       </c>
       <c r="T9" s="9">
         <f t="shared" si="0"/>
-        <v>44692</v>
+        <v>44657</v>
       </c>
       <c r="U9" s="9">
         <f t="shared" si="0"/>
-        <v>44693</v>
+        <v>44658</v>
       </c>
       <c r="V9" s="9">
         <f t="shared" si="0"/>
-        <v>44694</v>
+        <v>44659</v>
       </c>
       <c r="W9" s="9">
         <f t="shared" si="0"/>
-        <v>44695</v>
+        <v>44660</v>
       </c>
       <c r="X9" s="9">
         <f t="shared" si="0"/>
-        <v>44696</v>
+        <v>44661</v>
       </c>
       <c r="Y9" s="9">
         <f t="shared" si="0"/>
-        <v>44697</v>
+        <v>44662</v>
       </c>
       <c r="Z9" s="9">
         <f t="shared" si="0"/>
-        <v>44698</v>
+        <v>44663</v>
       </c>
       <c r="AA9" s="9">
         <f t="shared" si="0"/>
-        <v>44699</v>
+        <v>44664</v>
       </c>
       <c r="AB9" s="9">
         <f t="shared" si="0"/>
-        <v>44700</v>
+        <v>44665</v>
       </c>
       <c r="AC9" s="9">
         <f t="shared" si="0"/>
-        <v>44701</v>
+        <v>44666</v>
       </c>
       <c r="AD9" s="9">
         <f t="shared" si="0"/>
-        <v>44702</v>
+        <v>44667</v>
       </c>
       <c r="AE9" s="9">
         <f t="shared" si="0"/>
-        <v>44703</v>
+        <v>44668</v>
       </c>
       <c r="AF9" s="9">
         <f t="shared" si="0"/>
-        <v>44704</v>
+        <v>44669</v>
       </c>
       <c r="AG9" s="9">
         <f t="shared" si="0"/>
-        <v>44705</v>
+        <v>44670</v>
       </c>
       <c r="AH9" s="9">
         <f t="shared" si="0"/>
-        <v>44706</v>
+        <v>44671</v>
       </c>
       <c r="AI9" s="9">
         <f t="shared" si="0"/>
-        <v>44707</v>
+        <v>44672</v>
       </c>
       <c r="AJ9" s="9">
         <f t="shared" si="0"/>
-        <v>44708</v>
+        <v>44673</v>
       </c>
       <c r="AK9" s="9">
         <f t="shared" si="0"/>
-        <v>44709</v>
+        <v>44674</v>
       </c>
       <c r="AL9" s="9">
         <f t="shared" si="0"/>
-        <v>44710</v>
+        <v>44675</v>
       </c>
       <c r="AM9" s="9">
         <f t="shared" si="0"/>
-        <v>44711</v>
+        <v>44676</v>
       </c>
       <c r="AN9" s="9">
         <f t="shared" si="0"/>
-        <v>44712</v>
+        <v>44677</v>
       </c>
       <c r="AO9" s="9">
         <f t="shared" si="0"/>
-        <v>44713</v>
+        <v>44678</v>
       </c>
       <c r="AP9" s="9">
         <f t="shared" si="0"/>
-        <v>44714</v>
+        <v>44679</v>
       </c>
       <c r="AQ9" s="9">
         <f t="shared" si="0"/>
-        <v>44715</v>
+        <v>44680</v>
       </c>
       <c r="AR9" s="9">
         <f t="shared" si="0"/>
-        <v>44716</v>
+        <v>44681</v>
       </c>
       <c r="AS9" s="9">
         <f t="shared" si="0"/>
-        <v>44717</v>
+        <v>44682</v>
       </c>
       <c r="AT9" s="9">
         <f t="shared" si="0"/>
-        <v>44718</v>
+        <v>44683</v>
       </c>
       <c r="AU9" s="12">
         <f t="shared" si="0"/>
-        <v>44719</v>
+        <v>44684</v>
       </c>
     </row>
-    <row r="10" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C10" s="26">
         <v>1</v>
       </c>
@@ -8658,7 +8664,7 @@
       <c r="AT10" s="14"/>
       <c r="AU10" s="15"/>
     </row>
-    <row r="11" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C11" s="26">
         <v>2</v>
       </c>
@@ -8720,7 +8726,7 @@
       <c r="AT11" s="14"/>
       <c r="AU11" s="15"/>
     </row>
-    <row r="12" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C12" s="26">
         <v>3</v>
       </c>
@@ -8733,11 +8739,15 @@
       <c r="F12" s="7">
         <v>44683</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="7">
+        <v>44667</v>
+      </c>
+      <c r="H12" s="7">
+        <v>44669</v>
+      </c>
       <c r="I12" s="13">
         <f>COUNTIF(Steps!$G$11:$G$27,"true")/15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
@@ -8778,7 +8788,7 @@
       <c r="AT12" s="14"/>
       <c r="AU12" s="15"/>
     </row>
-    <row r="13" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C13" s="26">
         <v>4</v>
       </c>
@@ -8791,11 +8801,15 @@
       <c r="F13" s="7">
         <v>44684</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="7">
+        <v>44668</v>
+      </c>
+      <c r="H13" s="7">
+        <v>44670</v>
+      </c>
       <c r="I13" s="13">
         <f>COUNTIF(Steps!$G$29:$G$33,"true")/5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -8836,7 +8850,7 @@
       <c r="AT13" s="14"/>
       <c r="AU13" s="15"/>
     </row>
-    <row r="14" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C14" s="26">
         <v>5</v>
       </c>
@@ -8849,11 +8863,15 @@
       <c r="F14" s="7">
         <v>44685</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="G14" s="7">
+        <v>44669</v>
+      </c>
+      <c r="H14" s="7">
+        <v>44671</v>
+      </c>
       <c r="I14" s="13">
         <f>COUNTIF(Steps!$G$35:$G$39,"true")/5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
@@ -8894,7 +8912,7 @@
       <c r="AT14" s="14"/>
       <c r="AU14" s="15"/>
     </row>
-    <row r="15" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C15" s="26">
         <v>6</v>
       </c>
@@ -8907,11 +8925,15 @@
       <c r="F15" s="7">
         <v>44697</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="7">
+        <v>44670</v>
+      </c>
+      <c r="H15" s="7">
+        <v>44672</v>
+      </c>
       <c r="I15" s="13">
         <f>COUNTIF(Steps!$G$41:$G$43,"true")/3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
@@ -8952,7 +8974,7 @@
       <c r="AT15" s="14"/>
       <c r="AU15" s="15"/>
     </row>
-    <row r="16" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C16" s="26">
         <v>7</v>
       </c>
@@ -8965,11 +8987,15 @@
       <c r="F16" s="7">
         <v>44686</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="7">
+        <v>44671</v>
+      </c>
+      <c r="H16" s="7">
+        <v>44673</v>
+      </c>
       <c r="I16" s="13">
         <f>COUNTIF(Steps!$G$46:$G$57,"true")/10</f>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -9010,7 +9036,7 @@
       <c r="AT16" s="14"/>
       <c r="AU16" s="15"/>
     </row>
-    <row r="17" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C17" s="26">
         <v>8</v>
       </c>
@@ -9023,8 +9049,12 @@
       <c r="F17" s="7">
         <v>44687</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="7">
+        <v>44672</v>
+      </c>
+      <c r="H17" s="7">
+        <v>44674</v>
+      </c>
       <c r="I17" s="13">
         <f>COUNTIF(Steps!$G$60:$G$70,"true")/9</f>
         <v>0</v>
@@ -9068,7 +9098,7 @@
       <c r="AT17" s="14"/>
       <c r="AU17" s="15"/>
     </row>
-    <row r="18" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C18" s="26">
         <v>9</v>
       </c>
@@ -9081,8 +9111,12 @@
       <c r="F18" s="7">
         <v>44688</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="7">
+        <v>44673</v>
+      </c>
+      <c r="H18" s="7">
+        <v>44675</v>
+      </c>
       <c r="I18" s="13">
         <f>COUNTIF(Steps!$G$72,"true")/1</f>
         <v>0</v>
@@ -9126,7 +9160,7 @@
       <c r="AT18" s="14"/>
       <c r="AU18" s="15"/>
     </row>
-    <row r="19" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C19" s="26">
         <v>10</v>
       </c>
@@ -9139,8 +9173,12 @@
       <c r="F19" s="7">
         <v>44689</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="7">
+        <v>44674</v>
+      </c>
+      <c r="H19" s="7">
+        <v>44676</v>
+      </c>
       <c r="I19" s="13">
         <f>COUNTIF(Steps!$G$74:$G$76,"true")/3</f>
         <v>0</v>
@@ -9184,7 +9222,7 @@
       <c r="AT19" s="14"/>
       <c r="AU19" s="15"/>
     </row>
-    <row r="20" spans="3:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:47" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="34">
         <v>11</v>
       </c>
@@ -9197,8 +9235,12 @@
       <c r="F20" s="35">
         <v>44700</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
+      <c r="G20" s="7">
+        <v>44675</v>
+      </c>
+      <c r="H20" s="7">
+        <v>44677</v>
+      </c>
       <c r="I20" s="37">
         <f>COUNTIF(Steps!$G$78,"true")/1</f>
         <v>0</v>
@@ -9242,12 +9284,12 @@
       <c r="AT20" s="38"/>
       <c r="AU20" s="39"/>
     </row>
-    <row r="21" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:47" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="3:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:47" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -9414,17 +9456,17 @@
   </sheetPr>
   <dimension ref="D1:H78"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="136.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
+    <col min="5" max="5" width="136" customWidth="1"/>
+    <col min="6" max="6" width="10.09765625" customWidth="1"/>
+    <col min="7" max="7" width="8.796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:8" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
@@ -9438,17 +9480,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="89"/>
+      <c r="F2" s="83"/>
     </row>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D3" s="83"/>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="85"/>
       <c r="E3" s="27" t="s">
         <v>31</v>
       </c>
@@ -9458,8 +9500,8 @@
       </c>
       <c r="H3" s="40"/>
     </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D4" s="84"/>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="86"/>
       <c r="E4" s="27" t="s">
         <v>38</v>
       </c>
@@ -9468,27 +9510,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="85"/>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="87"/>
       <c r="E5" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="28" t="s">
+        <v>134</v>
+      </c>
       <c r="G5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D6" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="81" t="s">
+      <c r="E6" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="89"/>
+      <c r="F6" s="83"/>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D7" s="83"/>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="85"/>
       <c r="E7" s="28" t="s">
         <v>34</v>
       </c>
@@ -9497,8 +9541,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="85"/>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="87"/>
       <c r="E8" s="28" t="s">
         <v>35</v>
       </c>
@@ -9507,445 +9551,445 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D9" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="89"/>
+      <c r="F9" s="83"/>
     </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="83"/>
-      <c r="E10" s="79" t="s">
+    <row r="10" spans="4:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D10" s="85"/>
+      <c r="E10" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="90"/>
+      <c r="F10" s="84"/>
     </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="84"/>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="86"/>
       <c r="E11" s="29" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D12" s="84"/>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="86"/>
       <c r="E12" s="29" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D13" s="84"/>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="86"/>
       <c r="E13" s="29" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="28"/>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D14" s="84"/>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="86"/>
       <c r="E14" s="29" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D15" s="84"/>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="86"/>
       <c r="E15" s="29" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D16" s="84"/>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="86"/>
       <c r="E16" s="29" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="84"/>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="86"/>
       <c r="E17" s="29" t="s">
         <v>52</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="84"/>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="86"/>
       <c r="E18" s="29" t="s">
         <v>53</v>
       </c>
       <c r="F18" s="28"/>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="84"/>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="86"/>
       <c r="E19" s="29" t="s">
         <v>54</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="84"/>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20" s="86"/>
       <c r="E20" s="29" t="s">
         <v>55</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D21" s="84"/>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21" s="86"/>
       <c r="E21" s="29" t="s">
         <v>56</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="84"/>
+    <row r="22" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D22" s="86"/>
       <c r="E22" s="33" t="s">
         <v>57</v>
       </c>
       <c r="F22" s="32"/>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="84"/>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="86"/>
       <c r="E23" s="29" t="s">
         <v>58</v>
       </c>
       <c r="F23" s="28"/>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="84"/>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="86"/>
       <c r="E24" s="29" t="s">
         <v>59</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="84"/>
+    <row r="25" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D25" s="86"/>
       <c r="E25" s="33" t="s">
         <v>60</v>
       </c>
       <c r="F25" s="32"/>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" s="84"/>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="86"/>
       <c r="E26" s="28" t="s">
         <v>62</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D27" s="85"/>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="87"/>
       <c r="E27" s="28" t="s">
         <v>63</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D28" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="81" t="s">
+      <c r="E28" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="82"/>
+      <c r="F28" s="80"/>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="86"/>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="88"/>
       <c r="E29" s="28" t="s">
         <v>41</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="87"/>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="89"/>
       <c r="E30" s="28" t="s">
         <v>42</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D31" s="87"/>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="89"/>
       <c r="E31" s="28" t="s">
         <v>43</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D32" s="87"/>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="89"/>
       <c r="E32" s="28" t="s">
         <v>44</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D33" s="88"/>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D33" s="90"/>
       <c r="E33" s="28" t="s">
         <v>45</v>
       </c>
       <c r="F33" s="28"/>
       <c r="G33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D34" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="81" t="s">
+      <c r="E34" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="82"/>
+      <c r="F34" s="80"/>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D35" s="86"/>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D35" s="88"/>
       <c r="E35" s="28" t="s">
         <v>67</v>
       </c>
       <c r="F35" s="28"/>
       <c r="G35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D36" s="87"/>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D36" s="89"/>
       <c r="E36" s="28" t="s">
         <v>68</v>
       </c>
       <c r="F36" s="28"/>
       <c r="G36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="87"/>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D37" s="89"/>
       <c r="E37" s="28" t="s">
         <v>69</v>
       </c>
       <c r="F37" s="28"/>
       <c r="G37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D38" s="87"/>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D38" s="89"/>
       <c r="E38" s="28" t="s">
         <v>70</v>
       </c>
       <c r="F38" s="28"/>
       <c r="G38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D39" s="88"/>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D39" s="90"/>
       <c r="E39" s="28" t="s">
         <v>71</v>
       </c>
       <c r="F39" s="28"/>
       <c r="G39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D40" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E40" s="81" t="s">
+      <c r="E40" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="F40" s="82"/>
+      <c r="F40" s="80"/>
     </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D41" s="86"/>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D41" s="88"/>
       <c r="E41" s="28" t="s">
         <v>73</v>
       </c>
       <c r="F41" s="28"/>
       <c r="G41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D42" s="87"/>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="89"/>
       <c r="E42" s="28" t="s">
         <v>74</v>
       </c>
       <c r="F42" s="28"/>
       <c r="G42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D43" s="88"/>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="90"/>
       <c r="E43" s="28" t="s">
         <v>75</v>
       </c>
       <c r="F43" s="28"/>
       <c r="G43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D44" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="81" t="s">
+      <c r="E44" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="F44" s="82"/>
+      <c r="F44" s="80"/>
     </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D45" s="86"/>
-      <c r="E45" s="79" t="s">
+    <row r="45" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D45" s="88"/>
+      <c r="E45" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="F45" s="80"/>
+      <c r="F45" s="82"/>
     </row>
-    <row r="46" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D46" s="87"/>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D46" s="89"/>
       <c r="E46" s="28" t="s">
         <v>78</v>
       </c>
       <c r="F46" s="28"/>
       <c r="G46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="47" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D47" s="87"/>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="89"/>
       <c r="E47" s="28" t="s">
         <v>79</v>
       </c>
       <c r="F47" s="28"/>
       <c r="G47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="48" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D48" s="87"/>
+    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D48" s="89"/>
       <c r="E48" s="28" t="s">
         <v>80</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D49" s="87"/>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D49" s="89"/>
       <c r="E49" s="28" t="s">
         <v>81</v>
       </c>
       <c r="F49" s="28"/>
       <c r="G49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="50" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D50" s="87"/>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D50" s="89"/>
       <c r="E50" s="28" t="s">
         <v>82</v>
       </c>
       <c r="F50" s="28"/>
       <c r="G50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="51" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D51" s="87"/>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D51" s="89"/>
       <c r="E51" s="28" t="s">
         <v>83</v>
       </c>
       <c r="F51" s="28"/>
       <c r="G51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="52" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D52" s="87"/>
-      <c r="E52" s="79" t="s">
+    <row r="52" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D52" s="89"/>
+      <c r="E52" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="F52" s="80"/>
+      <c r="F52" s="82"/>
     </row>
-    <row r="53" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D53" s="87"/>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D53" s="89"/>
       <c r="E53" s="28" t="s">
         <v>86</v>
       </c>
       <c r="F53" s="28"/>
       <c r="G53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="54" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D54" s="87"/>
-      <c r="E54" s="79" t="s">
+    <row r="54" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D54" s="89"/>
+      <c r="E54" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="F54" s="80"/>
+      <c r="F54" s="82"/>
     </row>
-    <row r="55" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D55" s="87"/>
+    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D55" s="89"/>
       <c r="E55" s="28" t="s">
         <v>87</v>
       </c>
@@ -9954,8 +9998,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D56" s="87"/>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D56" s="89"/>
       <c r="E56" s="28" t="s">
         <v>89</v>
       </c>
@@ -9964,8 +10008,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D57" s="88"/>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D57" s="90"/>
       <c r="E57" s="28" t="s">
         <v>90</v>
       </c>
@@ -9974,23 +10018,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D58" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E58" s="81" t="s">
+      <c r="E58" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="F58" s="82"/>
+      <c r="F58" s="80"/>
     </row>
-    <row r="59" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D59" s="28"/>
-      <c r="E59" s="79" t="s">
+      <c r="E59" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="F59" s="80"/>
+      <c r="F59" s="82"/>
     </row>
-    <row r="60" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D60" s="28"/>
       <c r="E60" s="28" t="s">
         <v>94</v>
@@ -10000,7 +10044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D61" s="28"/>
       <c r="E61" s="28" t="s">
         <v>95</v>
@@ -10010,7 +10054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D62" s="28"/>
       <c r="E62" s="28" t="s">
         <v>96</v>
@@ -10020,7 +10064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D63" s="28"/>
       <c r="E63" s="28" t="s">
         <v>97</v>
@@ -10030,14 +10074,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D64" s="28"/>
-      <c r="E64" s="79" t="s">
+      <c r="E64" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="F64" s="80"/>
+      <c r="F64" s="82"/>
     </row>
-    <row r="65" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D65" s="28"/>
       <c r="E65" s="28" t="s">
         <v>99</v>
@@ -10047,7 +10091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D66" s="28"/>
       <c r="E66" s="28" t="s">
         <v>100</v>
@@ -10057,14 +10101,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D67" s="28"/>
-      <c r="E67" s="79" t="s">
+      <c r="E67" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="F67" s="80"/>
+      <c r="F67" s="82"/>
     </row>
-    <row r="68" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D68" s="28"/>
       <c r="E68" s="28" t="s">
         <v>102</v>
@@ -10074,7 +10118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D69" s="28"/>
       <c r="E69" s="28" t="s">
         <v>103</v>
@@ -10084,7 +10128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D70" s="28"/>
       <c r="E70" s="28" t="s">
         <v>104</v>
@@ -10094,16 +10138,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D71" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E71" s="81" t="s">
+      <c r="E71" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="F71" s="82"/>
+      <c r="F71" s="80"/>
     </row>
-    <row r="72" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D72" s="28"/>
       <c r="E72" s="28" t="s">
         <v>105</v>
@@ -10113,16 +10157,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D73" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="E73" s="81" t="s">
+      <c r="E73" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="F73" s="82"/>
+      <c r="F73" s="80"/>
     </row>
-    <row r="74" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D74" s="28"/>
       <c r="E74" s="28" t="s">
         <v>109</v>
@@ -10132,7 +10176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D75" s="28"/>
       <c r="E75" s="28" t="s">
         <v>110</v>
@@ -10142,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D76" s="28"/>
       <c r="E76" s="28" t="s">
         <v>111</v>
@@ -10152,16 +10196,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D77" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="E77" s="81" t="s">
+      <c r="E77" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="82"/>
+      <c r="F77" s="80"/>
     </row>
-    <row r="78" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D78" s="28"/>
       <c r="E78" s="28" t="s">
         <v>113</v>
@@ -10173,6 +10217,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D29:D33"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D45:D57"/>
+    <mergeCell ref="D10:D27"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E40:F40"/>
@@ -10186,18 +10242,6 @@
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="E54:F54"/>
     <mergeCell ref="E58:F58"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="D29:D33"/>
-    <mergeCell ref="D35:D39"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D45:D57"/>
-    <mergeCell ref="D10:D27"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E77:F77"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11715,122 +11759,123 @@
   <dimension ref="C1:AW28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6:Z6"/>
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.21875" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="49" width="3.21875" customWidth="1"/>
+    <col min="1" max="1" width="2.59765625" customWidth="1"/>
+    <col min="2" max="2" width="1.09765625" customWidth="1"/>
+    <col min="3" max="3" width="5.69921875" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" customWidth="1"/>
+    <col min="5" max="5" width="4.09765625" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="10" width="7.09765625" customWidth="1"/>
+    <col min="11" max="11" width="3.796875" customWidth="1"/>
+    <col min="12" max="49" width="3.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:49" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="101"/>
-      <c r="Y1" s="101"/>
-      <c r="Z1" s="101"/>
-      <c r="AA1" s="101"/>
-      <c r="AB1" s="101"/>
-      <c r="AC1" s="101"/>
-      <c r="AD1" s="101"/>
-      <c r="AE1" s="101"/>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="101"/>
-      <c r="AH1" s="101"/>
-      <c r="AI1" s="101"/>
-      <c r="AJ1" s="101"/>
-      <c r="AK1" s="101"/>
-      <c r="AL1" s="101"/>
-      <c r="AM1" s="101"/>
-      <c r="AN1" s="101"/>
-      <c r="AO1" s="101"/>
-      <c r="AP1" s="101"/>
-      <c r="AQ1" s="101"/>
-      <c r="AR1" s="101"/>
-      <c r="AS1" s="101"/>
-      <c r="AT1" s="101"/>
-      <c r="AU1" s="101"/>
-      <c r="AV1" s="101"/>
-      <c r="AW1" s="101"/>
+    <row r="1" spans="3:49" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="92"/>
+      <c r="AI1" s="92"/>
+      <c r="AJ1" s="92"/>
+      <c r="AK1" s="92"/>
+      <c r="AL1" s="92"/>
+      <c r="AM1" s="92"/>
+      <c r="AN1" s="92"/>
+      <c r="AO1" s="92"/>
+      <c r="AP1" s="92"/>
+      <c r="AQ1" s="92"/>
+      <c r="AR1" s="92"/>
+      <c r="AS1" s="92"/>
+      <c r="AT1" s="92"/>
+      <c r="AU1" s="92"/>
+      <c r="AV1" s="92"/>
+      <c r="AW1" s="92"/>
     </row>
-    <row r="2" spans="3:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101"/>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="101"/>
-      <c r="W2" s="101"/>
-      <c r="X2" s="101"/>
-      <c r="Y2" s="101"/>
-      <c r="Z2" s="101"/>
-      <c r="AA2" s="101"/>
-      <c r="AB2" s="101"/>
-      <c r="AC2" s="101"/>
-      <c r="AD2" s="101"/>
-      <c r="AE2" s="101"/>
-      <c r="AF2" s="101"/>
-      <c r="AG2" s="101"/>
-      <c r="AH2" s="101"/>
-      <c r="AI2" s="101"/>
-      <c r="AJ2" s="101"/>
-      <c r="AK2" s="101"/>
-      <c r="AL2" s="101"/>
-      <c r="AM2" s="101"/>
-      <c r="AN2" s="101"/>
-      <c r="AO2" s="101"/>
-      <c r="AP2" s="101"/>
-      <c r="AQ2" s="101"/>
-      <c r="AR2" s="101"/>
-      <c r="AS2" s="101"/>
-      <c r="AT2" s="101"/>
-      <c r="AU2" s="101"/>
-      <c r="AV2" s="101"/>
-      <c r="AW2" s="101"/>
+    <row r="2" spans="3:49" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="92"/>
+      <c r="AA2" s="92"/>
+      <c r="AB2" s="92"/>
+      <c r="AC2" s="92"/>
+      <c r="AD2" s="92"/>
+      <c r="AE2" s="92"/>
+      <c r="AF2" s="92"/>
+      <c r="AG2" s="92"/>
+      <c r="AH2" s="92"/>
+      <c r="AI2" s="92"/>
+      <c r="AJ2" s="92"/>
+      <c r="AK2" s="92"/>
+      <c r="AL2" s="92"/>
+      <c r="AM2" s="92"/>
+      <c r="AN2" s="92"/>
+      <c r="AO2" s="92"/>
+      <c r="AP2" s="92"/>
+      <c r="AQ2" s="92"/>
+      <c r="AR2" s="92"/>
+      <c r="AS2" s="92"/>
+      <c r="AT2" s="92"/>
+      <c r="AU2" s="92"/>
+      <c r="AV2" s="92"/>
+      <c r="AW2" s="92"/>
     </row>
-    <row r="3" spans="3:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C3" s="65" t="s">
         <v>23</v>
       </c>
@@ -11881,7 +11926,7 @@
       <c r="AV3" s="66"/>
       <c r="AW3" s="67"/>
     </row>
-    <row r="4" spans="3:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:49" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="68"/>
       <c r="D4" s="69"/>
       <c r="E4" s="69"/>
@@ -11930,13 +11975,13 @@
       <c r="AV4" s="69"/>
       <c r="AW4" s="70"/>
     </row>
-    <row r="5" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C5" s="102" t="s">
+    <row r="5" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C5" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="104"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="95"/>
       <c r="G5" s="18">
         <f ca="1">TODAY()</f>
         <v>44699</v>
@@ -11988,13 +12033,13 @@
       <c r="AV5" s="5"/>
       <c r="AW5" s="10"/>
     </row>
-    <row r="6" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C6" s="105" t="s">
+    <row r="6" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C6" s="96" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="107"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98"/>
       <c r="G6" s="4" t="s">
         <v>130</v>
       </c>
@@ -12049,7 +12094,7 @@
       <c r="AV6" s="5"/>
       <c r="AW6" s="10"/>
     </row>
-    <row r="7" spans="3:49" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:49" x14ac:dyDescent="0.25">
       <c r="C7" s="25"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -12098,32 +12143,32 @@
       <c r="AV7" s="5"/>
       <c r="AW7" s="10"/>
     </row>
-    <row r="8" spans="3:49" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="108" t="s">
+    <row r="8" spans="3:49" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="100" t="s">
+      <c r="D8" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="100" t="s">
+      <c r="E8" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="100" t="s">
+      <c r="F8" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="100" t="s">
+      <c r="G8" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="100" t="s">
+      <c r="H8" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="100" t="s">
+      <c r="I8" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="100" t="s">
+      <c r="J8" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="100" t="s">
+      <c r="K8" s="91" t="s">
         <v>17</v>
       </c>
       <c r="L8" s="44" t="s">
@@ -12241,16 +12286,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C9" s="108"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="100"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="100"/>
+    <row r="9" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C9" s="99"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
       <c r="L9" s="47">
         <f>DATE($X$6,$AF$6,1)-WEEKDAY(DATE($X$6,$AF$6,1),1)+1</f>
         <v>44682</v>
@@ -12404,8 +12449,8 @@
         <v>44719</v>
       </c>
     </row>
-    <row r="10" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C10" s="91" t="s">
+    <row r="10" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C10" s="100" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="49" t="s">
@@ -12414,7 +12459,7 @@
       <c r="E10" s="50">
         <v>28</v>
       </c>
-      <c r="F10" s="93">
+      <c r="F10" s="102">
         <v>2</v>
       </c>
       <c r="G10" s="51">
@@ -12467,15 +12512,15 @@
       <c r="AV10" s="42"/>
       <c r="AW10" s="20"/>
     </row>
-    <row r="11" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C11" s="92"/>
+    <row r="11" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C11" s="101"/>
       <c r="D11" s="49" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="50">
         <v>18</v>
       </c>
-      <c r="F11" s="94"/>
+      <c r="F11" s="103"/>
       <c r="G11" s="51">
         <v>44698</v>
       </c>
@@ -12526,16 +12571,16 @@
       <c r="AV11" s="42"/>
       <c r="AW11" s="20"/>
     </row>
-    <row r="12" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="95"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="97"/>
+    <row r="12" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="104"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
+      <c r="K12" s="106"/>
       <c r="L12" s="42"/>
       <c r="M12" s="42"/>
       <c r="N12" s="42"/>
@@ -12575,8 +12620,8 @@
       <c r="AV12" s="42"/>
       <c r="AW12" s="20"/>
     </row>
-    <row r="13" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C13" s="91" t="s">
+    <row r="13" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C13" s="100" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="49" t="s">
@@ -12585,7 +12630,7 @@
       <c r="E13" s="50">
         <v>24</v>
       </c>
-      <c r="F13" s="93">
+      <c r="F13" s="102">
         <v>2</v>
       </c>
       <c r="G13" s="51">
@@ -12638,15 +12683,15 @@
       <c r="AV13" s="42"/>
       <c r="AW13" s="20"/>
     </row>
-    <row r="14" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C14" s="92"/>
+    <row r="14" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C14" s="101"/>
       <c r="D14" s="49" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="50">
         <v>17</v>
       </c>
-      <c r="F14" s="94"/>
+      <c r="F14" s="103"/>
       <c r="G14" s="51">
         <v>44698</v>
       </c>
@@ -12697,16 +12742,16 @@
       <c r="AV14" s="42"/>
       <c r="AW14" s="20"/>
     </row>
-    <row r="15" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="95"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="96"/>
-      <c r="H15" s="96"/>
-      <c r="I15" s="96"/>
-      <c r="J15" s="96"/>
-      <c r="K15" s="97"/>
+    <row r="15" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="104"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="106"/>
       <c r="L15" s="42"/>
       <c r="M15" s="42"/>
       <c r="N15" s="42"/>
@@ -12746,8 +12791,8 @@
       <c r="AV15" s="42"/>
       <c r="AW15" s="20"/>
     </row>
-    <row r="16" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C16" s="91" t="s">
+    <row r="16" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C16" s="100" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="49" t="s">
@@ -12756,7 +12801,7 @@
       <c r="E16" s="50">
         <v>19</v>
       </c>
-      <c r="F16" s="93">
+      <c r="F16" s="102">
         <v>1</v>
       </c>
       <c r="G16" s="51">
@@ -12809,15 +12854,15 @@
       <c r="AV16" s="42"/>
       <c r="AW16" s="20"/>
     </row>
-    <row r="17" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C17" s="92"/>
+    <row r="17" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C17" s="101"/>
       <c r="D17" s="49" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="50">
         <v>17</v>
       </c>
-      <c r="F17" s="94"/>
+      <c r="F17" s="103"/>
       <c r="G17" s="51">
         <v>44698</v>
       </c>
@@ -12868,16 +12913,16 @@
       <c r="AV17" s="42"/>
       <c r="AW17" s="20"/>
     </row>
-    <row r="18" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="95"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="97"/>
+    <row r="18" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="104"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="106"/>
       <c r="L18" s="42"/>
       <c r="M18" s="42"/>
       <c r="N18" s="42"/>
@@ -12917,8 +12962,8 @@
       <c r="AV18" s="42"/>
       <c r="AW18" s="20"/>
     </row>
-    <row r="19" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C19" s="91" t="s">
+    <row r="19" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C19" s="100" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="49" t="s">
@@ -12927,7 +12972,7 @@
       <c r="E19" s="50">
         <v>22</v>
       </c>
-      <c r="F19" s="93">
+      <c r="F19" s="102">
         <v>1</v>
       </c>
       <c r="G19" s="51">
@@ -12980,15 +13025,15 @@
       <c r="AV19" s="42"/>
       <c r="AW19" s="20"/>
     </row>
-    <row r="20" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C20" s="92"/>
+    <row r="20" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C20" s="101"/>
       <c r="D20" s="49" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="50">
         <v>17</v>
       </c>
-      <c r="F20" s="94"/>
+      <c r="F20" s="103"/>
       <c r="G20" s="51">
         <v>44698</v>
       </c>
@@ -13039,7 +13084,7 @@
       <c r="AV20" s="42"/>
       <c r="AW20" s="20"/>
     </row>
-    <row r="21" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="53"/>
       <c r="D21" s="54"/>
       <c r="E21" s="55"/>
@@ -13088,8 +13133,8 @@
       <c r="AV21" s="42"/>
       <c r="AW21" s="20"/>
     </row>
-    <row r="22" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C22" s="91" t="s">
+    <row r="22" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C22" s="100" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="49" t="s">
@@ -13098,7 +13143,7 @@
       <c r="E22" s="50">
         <v>0</v>
       </c>
-      <c r="F22" s="93">
+      <c r="F22" s="102">
         <v>0</v>
       </c>
       <c r="G22" s="51"/>
@@ -13147,15 +13192,15 @@
       <c r="AV22" s="42"/>
       <c r="AW22" s="20"/>
     </row>
-    <row r="23" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C23" s="92"/>
+    <row r="23" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C23" s="101"/>
       <c r="D23" s="49" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="50">
         <v>0</v>
       </c>
-      <c r="F23" s="94"/>
+      <c r="F23" s="103"/>
       <c r="G23" s="51"/>
       <c r="H23" s="51"/>
       <c r="I23" s="51"/>
@@ -13202,16 +13247,16 @@
       <c r="AV23" s="42"/>
       <c r="AW23" s="20"/>
     </row>
-    <row r="24" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="95"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="96"/>
-      <c r="G24" s="96"/>
-      <c r="H24" s="96"/>
-      <c r="I24" s="96"/>
-      <c r="J24" s="96"/>
-      <c r="K24" s="97"/>
+    <row r="24" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="104"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="106"/>
       <c r="L24" s="42"/>
       <c r="M24" s="42"/>
       <c r="N24" s="42"/>
@@ -13251,8 +13296,8 @@
       <c r="AV24" s="42"/>
       <c r="AW24" s="20"/>
     </row>
-    <row r="25" spans="3:49" x14ac:dyDescent="0.3">
-      <c r="C25" s="91" t="s">
+    <row r="25" spans="3:49" x14ac:dyDescent="0.25">
+      <c r="C25" s="100" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="49" t="s">
@@ -13261,7 +13306,7 @@
       <c r="E25" s="50">
         <v>11</v>
       </c>
-      <c r="F25" s="93">
+      <c r="F25" s="102">
         <v>1</v>
       </c>
       <c r="G25" s="51">
@@ -13314,15 +13359,15 @@
       <c r="AV25" s="42"/>
       <c r="AW25" s="20"/>
     </row>
-    <row r="26" spans="3:49" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="98"/>
+    <row r="26" spans="3:49" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="107"/>
       <c r="D26" s="59" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="60">
         <v>11</v>
       </c>
-      <c r="F26" s="99"/>
+      <c r="F26" s="108"/>
       <c r="G26" s="61">
         <v>44698</v>
       </c>
@@ -13373,14 +13418,14 @@
       <c r="AV26" s="21"/>
       <c r="AW26" s="22"/>
     </row>
-    <row r="27" spans="3:49" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:49" x14ac:dyDescent="0.25">
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="3:49" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:49" x14ac:dyDescent="0.25">
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -13389,6 +13434,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="C24:K24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F13:F14"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
@@ -13405,22 +13466,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C15:K15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="C24:K24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="F25:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="L9:AW9">
     <cfRule type="expression" dxfId="8" priority="4">
@@ -13464,12 +13509,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6:Z6">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>YEAR(TODAY())=$X$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF6">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(YEAR(TODAY())=$X$6,MONTH(TODAY())=$AF$6)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update By Shiping V1.2
</commit_message>
<xml_diff>
--- a/ClusterTraining.xlsx
+++ b/ClusterTraining.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT PROJECTS\Shipin3x\Shipin3x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8108335-8DBA-49E7-B359-A096E0D59CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B1BFC3-FB1B-4667-AF83-5F337B7356EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClusterTrainingSchedule" sheetId="1" r:id="rId1"/>
@@ -1150,6 +1150,18 @@
     <xf numFmtId="9" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1285,23 +1297,32 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+        <right style="thin">
+          <color theme="7"/>
+        </right>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1347,27 +1368,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFFF0000"/>
@@ -1387,18 +1387,10 @@
         </patternFill>
       </fill>
       <border>
-        <left style="dotted">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="dotted">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="dotted">
-          <color rgb="FF00B050"/>
-        </top>
-        <bottom style="dotted">
-          <color rgb="FF00B050"/>
-        </bottom>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1526,6 +1518,122 @@
         </right>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightGray">
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF0000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="dotted">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="dotted">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="dotted">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1584,7 +1692,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$AD$6" max="12" min="1" page="10" val="5"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$AD$6" max="12" min="1" page="10" val="4"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7957,8 +8065,8 @@
   </sheetPr>
   <dimension ref="C1:AU22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7976,200 +8084,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:47" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
-      <c r="AD1" s="61"/>
-      <c r="AE1" s="61"/>
-      <c r="AF1" s="61"/>
-      <c r="AG1" s="61"/>
-      <c r="AH1" s="61"/>
-      <c r="AI1" s="61"/>
-      <c r="AJ1" s="61"/>
-      <c r="AK1" s="61"/>
-      <c r="AL1" s="61"/>
-      <c r="AM1" s="61"/>
-      <c r="AN1" s="61"/>
-      <c r="AO1" s="61"/>
-      <c r="AP1" s="61"/>
-      <c r="AQ1" s="61"/>
-      <c r="AR1" s="61"/>
-      <c r="AS1" s="61"/>
-      <c r="AT1" s="61"/>
-      <c r="AU1" s="61"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
     </row>
     <row r="2" spans="3:47" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="61"/>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="61"/>
-      <c r="AE2" s="61"/>
-      <c r="AF2" s="61"/>
-      <c r="AG2" s="61"/>
-      <c r="AH2" s="61"/>
-      <c r="AI2" s="61"/>
-      <c r="AJ2" s="61"/>
-      <c r="AK2" s="61"/>
-      <c r="AL2" s="61"/>
-      <c r="AM2" s="61"/>
-      <c r="AN2" s="61"/>
-      <c r="AO2" s="61"/>
-      <c r="AP2" s="61"/>
-      <c r="AQ2" s="61"/>
-      <c r="AR2" s="61"/>
-      <c r="AS2" s="61"/>
-      <c r="AT2" s="61"/>
-      <c r="AU2" s="61"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="65"/>
+      <c r="AJ2" s="65"/>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="65"/>
     </row>
     <row r="3" spans="3:47" x14ac:dyDescent="0.25">
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="63"/>
-      <c r="AD3" s="63"/>
-      <c r="AE3" s="63"/>
-      <c r="AF3" s="63"/>
-      <c r="AG3" s="63"/>
-      <c r="AH3" s="63"/>
-      <c r="AI3" s="63"/>
-      <c r="AJ3" s="63"/>
-      <c r="AK3" s="63"/>
-      <c r="AL3" s="63"/>
-      <c r="AM3" s="63"/>
-      <c r="AN3" s="63"/>
-      <c r="AO3" s="63"/>
-      <c r="AP3" s="63"/>
-      <c r="AQ3" s="63"/>
-      <c r="AR3" s="63"/>
-      <c r="AS3" s="63"/>
-      <c r="AT3" s="63"/>
-      <c r="AU3" s="64"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
+      <c r="AJ3" s="67"/>
+      <c r="AK3" s="67"/>
+      <c r="AL3" s="67"/>
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="68"/>
     </row>
     <row r="4" spans="3:47" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="66"/>
-      <c r="W4" s="66"/>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="66"/>
-      <c r="AG4" s="66"/>
-      <c r="AH4" s="66"/>
-      <c r="AI4" s="66"/>
-      <c r="AJ4" s="66"/>
-      <c r="AK4" s="66"/>
-      <c r="AL4" s="66"/>
-      <c r="AM4" s="66"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="66"/>
-      <c r="AQ4" s="66"/>
-      <c r="AR4" s="66"/>
-      <c r="AS4" s="66"/>
-      <c r="AT4" s="66"/>
-      <c r="AU4" s="67"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="70"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="70"/>
+      <c r="AD4" s="70"/>
+      <c r="AE4" s="70"/>
+      <c r="AF4" s="70"/>
+      <c r="AG4" s="70"/>
+      <c r="AH4" s="70"/>
+      <c r="AI4" s="70"/>
+      <c r="AJ4" s="70"/>
+      <c r="AK4" s="70"/>
+      <c r="AL4" s="70"/>
+      <c r="AM4" s="70"/>
+      <c r="AN4" s="70"/>
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="70"/>
+      <c r="AQ4" s="70"/>
+      <c r="AR4" s="70"/>
+      <c r="AS4" s="70"/>
+      <c r="AT4" s="70"/>
+      <c r="AU4" s="71"/>
     </row>
     <row r="5" spans="3:47" x14ac:dyDescent="0.25">
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="69"/>
+      <c r="D5" s="73"/>
       <c r="E5" s="17">
         <f ca="1">TODAY()</f>
         <v>44700</v>
@@ -8222,10 +8330,10 @@
       <c r="AU5" s="9"/>
     </row>
     <row r="6" spans="3:47" x14ac:dyDescent="0.25">
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="71"/>
+      <c r="D6" s="75"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -8241,24 +8349,24 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
-      <c r="T6" s="75" t="s">
+      <c r="T6" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="U6" s="75"/>
-      <c r="V6" s="74">
+      <c r="U6" s="79"/>
+      <c r="V6" s="78">
         <v>2022</v>
       </c>
-      <c r="W6" s="74"/>
-      <c r="X6" s="74"/>
+      <c r="W6" s="78"/>
+      <c r="X6" s="78"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="75" t="s">
+      <c r="AA6" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="AB6" s="75"/>
-      <c r="AC6" s="75"/>
+      <c r="AB6" s="79"/>
+      <c r="AC6" s="79"/>
       <c r="AD6" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE6" s="5"/>
       <c r="AF6" s="5"/>
@@ -8326,25 +8434,25 @@
       <c r="AU7" s="9"/>
     </row>
     <row r="8" spans="3:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="72" t="s">
+      <c r="E8" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="72" t="s">
+      <c r="F8" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="72" t="s">
+      <c r="G8" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="I8" s="72" t="s">
+      <c r="I8" s="76" t="s">
         <v>17</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -8463,164 +8571,164 @@
       </c>
     </row>
     <row r="9" spans="3:47" x14ac:dyDescent="0.25">
-      <c r="C9" s="73"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
       <c r="J9" s="8">
         <f>DATE($V$6,$AD$6,1)-WEEKDAY(DATE($V$6,$AD$6,1),1)+1</f>
-        <v>44682</v>
+        <v>44647</v>
       </c>
       <c r="K9" s="8">
         <f>J9+1</f>
-        <v>44683</v>
+        <v>44648</v>
       </c>
       <c r="L9" s="8">
         <f t="shared" ref="L9:AU9" si="0">K9+1</f>
-        <v>44684</v>
+        <v>44649</v>
       </c>
       <c r="M9" s="8">
         <f t="shared" si="0"/>
-        <v>44685</v>
+        <v>44650</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" si="0"/>
-        <v>44686</v>
+        <v>44651</v>
       </c>
       <c r="O9" s="8">
         <f t="shared" si="0"/>
-        <v>44687</v>
+        <v>44652</v>
       </c>
       <c r="P9" s="8">
         <f t="shared" si="0"/>
-        <v>44688</v>
+        <v>44653</v>
       </c>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>44689</v>
+        <v>44654</v>
       </c>
       <c r="R9" s="8">
         <f t="shared" si="0"/>
-        <v>44690</v>
+        <v>44655</v>
       </c>
       <c r="S9" s="8">
         <f t="shared" si="0"/>
-        <v>44691</v>
+        <v>44656</v>
       </c>
       <c r="T9" s="8">
         <f t="shared" si="0"/>
-        <v>44692</v>
+        <v>44657</v>
       </c>
       <c r="U9" s="8">
         <f t="shared" si="0"/>
-        <v>44693</v>
+        <v>44658</v>
       </c>
       <c r="V9" s="8">
         <f t="shared" si="0"/>
-        <v>44694</v>
+        <v>44659</v>
       </c>
       <c r="W9" s="8">
         <f t="shared" si="0"/>
-        <v>44695</v>
+        <v>44660</v>
       </c>
       <c r="X9" s="8">
         <f t="shared" si="0"/>
-        <v>44696</v>
+        <v>44661</v>
       </c>
       <c r="Y9" s="8">
         <f t="shared" si="0"/>
-        <v>44697</v>
+        <v>44662</v>
       </c>
       <c r="Z9" s="8">
         <f t="shared" si="0"/>
-        <v>44698</v>
+        <v>44663</v>
       </c>
       <c r="AA9" s="8">
         <f t="shared" si="0"/>
-        <v>44699</v>
+        <v>44664</v>
       </c>
       <c r="AB9" s="8">
         <f t="shared" si="0"/>
-        <v>44700</v>
+        <v>44665</v>
       </c>
       <c r="AC9" s="8">
         <f t="shared" si="0"/>
-        <v>44701</v>
+        <v>44666</v>
       </c>
       <c r="AD9" s="8">
         <f t="shared" si="0"/>
-        <v>44702</v>
+        <v>44667</v>
       </c>
       <c r="AE9" s="8">
         <f t="shared" si="0"/>
-        <v>44703</v>
+        <v>44668</v>
       </c>
       <c r="AF9" s="8">
         <f t="shared" si="0"/>
-        <v>44704</v>
+        <v>44669</v>
       </c>
       <c r="AG9" s="8">
         <f t="shared" si="0"/>
-        <v>44705</v>
+        <v>44670</v>
       </c>
       <c r="AH9" s="8">
         <f t="shared" si="0"/>
-        <v>44706</v>
+        <v>44671</v>
       </c>
       <c r="AI9" s="8">
         <f t="shared" si="0"/>
-        <v>44707</v>
+        <v>44672</v>
       </c>
       <c r="AJ9" s="8">
         <f t="shared" si="0"/>
-        <v>44708</v>
+        <v>44673</v>
       </c>
       <c r="AK9" s="8">
         <f t="shared" si="0"/>
-        <v>44709</v>
+        <v>44674</v>
       </c>
       <c r="AL9" s="8">
         <f t="shared" si="0"/>
-        <v>44710</v>
+        <v>44675</v>
       </c>
       <c r="AM9" s="8">
         <f t="shared" si="0"/>
-        <v>44711</v>
+        <v>44676</v>
       </c>
       <c r="AN9" s="8">
         <f t="shared" si="0"/>
-        <v>44712</v>
+        <v>44677</v>
       </c>
       <c r="AO9" s="8">
         <f t="shared" si="0"/>
-        <v>44713</v>
+        <v>44678</v>
       </c>
       <c r="AP9" s="8">
         <f t="shared" si="0"/>
-        <v>44714</v>
+        <v>44679</v>
       </c>
       <c r="AQ9" s="8">
         <f t="shared" si="0"/>
-        <v>44715</v>
+        <v>44680</v>
       </c>
       <c r="AR9" s="8">
         <f t="shared" si="0"/>
-        <v>44716</v>
+        <v>44681</v>
       </c>
       <c r="AS9" s="8">
         <f t="shared" si="0"/>
-        <v>44717</v>
+        <v>44682</v>
       </c>
       <c r="AT9" s="8">
         <f t="shared" si="0"/>
-        <v>44718</v>
+        <v>44683</v>
       </c>
       <c r="AU9" s="11">
         <f t="shared" si="0"/>
-        <v>44719</v>
+        <v>44684</v>
       </c>
     </row>
     <row r="10" spans="3:47" x14ac:dyDescent="0.25">
@@ -8630,17 +8738,17 @@
       <c r="D10" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="106">
+      <c r="E10" s="61">
         <v>44663</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F10" s="61">
         <v>44667</v>
       </c>
-      <c r="G10" s="109">
+      <c r="G10" s="64">
         <v>44663</v>
       </c>
-      <c r="H10" s="109">
-        <v>44665</v>
+      <c r="H10" s="64">
+        <v>44678</v>
       </c>
       <c r="I10" s="12">
         <f>COUNTIF(Steps!$G$3:$G$5,"true")/3</f>
@@ -8692,16 +8800,16 @@
       <c r="D11" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="106">
+      <c r="E11" s="61">
         <v>44668</v>
       </c>
-      <c r="F11" s="106">
+      <c r="F11" s="61">
         <v>44670</v>
       </c>
-      <c r="G11" s="109">
+      <c r="G11" s="64">
         <v>44666</v>
       </c>
-      <c r="H11" s="109">
+      <c r="H11" s="64">
         <v>44668</v>
       </c>
       <c r="I11" s="12">
@@ -8754,16 +8862,16 @@
       <c r="D12" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="106">
+      <c r="E12" s="61">
         <v>44671</v>
       </c>
-      <c r="F12" s="106">
+      <c r="F12" s="61">
         <v>44683</v>
       </c>
-      <c r="G12" s="109">
+      <c r="G12" s="64">
         <v>44667</v>
       </c>
-      <c r="H12" s="109">
+      <c r="H12" s="64">
         <v>44669</v>
       </c>
       <c r="I12" s="12">
@@ -8816,16 +8924,16 @@
       <c r="D13" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="106">
+      <c r="E13" s="61">
         <v>44659</v>
       </c>
-      <c r="F13" s="106">
+      <c r="F13" s="61">
         <v>44684</v>
       </c>
-      <c r="G13" s="109">
+      <c r="G13" s="64">
         <v>44668</v>
       </c>
-      <c r="H13" s="109">
+      <c r="H13" s="64">
         <v>44670</v>
       </c>
       <c r="I13" s="12">
@@ -8878,16 +8986,16 @@
       <c r="D14" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="E14" s="106">
+      <c r="E14" s="61">
         <v>44660</v>
       </c>
-      <c r="F14" s="106">
+      <c r="F14" s="61">
         <v>44685</v>
       </c>
-      <c r="G14" s="109">
+      <c r="G14" s="64">
         <v>44669</v>
       </c>
-      <c r="H14" s="109">
+      <c r="H14" s="64">
         <v>44671</v>
       </c>
       <c r="I14" s="12">
@@ -8940,16 +9048,16 @@
       <c r="D15" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E15" s="106">
+      <c r="E15" s="61">
         <v>44697</v>
       </c>
-      <c r="F15" s="106">
+      <c r="F15" s="61">
         <v>44697</v>
       </c>
-      <c r="G15" s="109">
+      <c r="G15" s="64">
         <v>44670</v>
       </c>
-      <c r="H15" s="109">
+      <c r="H15" s="64">
         <v>44672</v>
       </c>
       <c r="I15" s="12">
@@ -9002,16 +9110,16 @@
       <c r="D16" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="E16" s="106">
+      <c r="E16" s="61">
         <v>44669</v>
       </c>
-      <c r="F16" s="106">
+      <c r="F16" s="61">
         <v>44686</v>
       </c>
-      <c r="G16" s="109">
+      <c r="G16" s="64">
         <v>44671</v>
       </c>
-      <c r="H16" s="109">
+      <c r="H16" s="64">
         <v>44673</v>
       </c>
       <c r="I16" s="12">
@@ -9064,16 +9172,16 @@
       <c r="D17" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="E17" s="106">
+      <c r="E17" s="61">
         <v>44662</v>
       </c>
-      <c r="F17" s="106">
+      <c r="F17" s="61">
         <v>44687</v>
       </c>
-      <c r="G17" s="109">
+      <c r="G17" s="64">
         <v>44672</v>
       </c>
-      <c r="H17" s="109">
+      <c r="H17" s="64">
         <v>44674</v>
       </c>
       <c r="I17" s="12">
@@ -9126,16 +9234,16 @@
       <c r="D18" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="106">
+      <c r="E18" s="61">
         <v>44663</v>
       </c>
-      <c r="F18" s="106">
+      <c r="F18" s="61">
         <v>44688</v>
       </c>
-      <c r="G18" s="109">
+      <c r="G18" s="64">
         <v>44673</v>
       </c>
-      <c r="H18" s="109">
+      <c r="H18" s="64">
         <v>44675</v>
       </c>
       <c r="I18" s="12">
@@ -9188,16 +9296,16 @@
       <c r="D19" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="106">
+      <c r="E19" s="61">
         <v>44664</v>
       </c>
-      <c r="F19" s="106">
+      <c r="F19" s="61">
         <v>44689</v>
       </c>
-      <c r="G19" s="109">
+      <c r="G19" s="64">
         <v>44674</v>
       </c>
-      <c r="H19" s="109">
+      <c r="H19" s="64">
         <v>44676</v>
       </c>
       <c r="I19" s="12">
@@ -9250,16 +9358,16 @@
       <c r="D20" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="107">
+      <c r="E20" s="62">
         <v>44665</v>
       </c>
-      <c r="F20" s="108">
+      <c r="F20" s="63">
         <v>44700</v>
       </c>
-      <c r="G20" s="109">
-        <v>44675</v>
-      </c>
-      <c r="H20" s="109">
+      <c r="G20" s="64">
+        <v>44644</v>
+      </c>
+      <c r="H20" s="64">
         <v>44700</v>
       </c>
       <c r="I20" s="34">
@@ -9334,10 +9442,10 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J9:AU9">
-    <cfRule type="expression" dxfId="17" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>AND(YEAR(TODAY())=$V$6,MONTH(TODAY())=$AD$6,DAY(J9)=DAY(TODAY()),MONTH(J9)=$AD$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>MONTH(J9)&lt;&gt;$AD$6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9356,31 +9464,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:AU20">
-    <cfRule type="expression" dxfId="15" priority="12">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>AND(J$9&gt;=$G10,J$9&lt;=$H10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="5" priority="13">
       <formula>J$9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>AND(J$9&gt;=$E10,J$9&lt;=$F10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="4" priority="15">
       <formula>K$9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="16">
+    <cfRule type="expression" dxfId="3" priority="16">
       <formula>AND(K$9&gt;=$E6,K$9&lt;=$F6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V6:X6">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>YEAR(TODAY())=$V$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD6">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(YEAR(TODAY())=$V$6,MONTH(TODAY())=$AD$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9505,13 +9613,13 @@
       <c r="D2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="76" t="s">
+      <c r="E2" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="80"/>
+      <c r="F2" s="84"/>
     </row>
     <row r="3" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="82"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="26" t="s">
         <v>31</v>
       </c>
@@ -9522,7 +9630,7 @@
       <c r="H3" s="37"/>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="83"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="26" t="s">
         <v>38</v>
       </c>
@@ -9532,7 +9640,7 @@
       </c>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="84"/>
+      <c r="D5" s="88"/>
       <c r="E5" s="27" t="s">
         <v>132</v>
       </c>
@@ -9547,13 +9655,13 @@
       <c r="D6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="80"/>
+      <c r="F6" s="84"/>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="82"/>
+      <c r="D7" s="86"/>
       <c r="E7" s="27" t="s">
         <v>34</v>
       </c>
@@ -9563,7 +9671,7 @@
       </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="84"/>
+      <c r="D8" s="88"/>
       <c r="E8" s="27" t="s">
         <v>35</v>
       </c>
@@ -9576,20 +9684,20 @@
       <c r="D9" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="80"/>
+      <c r="F9" s="84"/>
     </row>
     <row r="10" spans="4:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D10" s="82"/>
-      <c r="E10" s="78" t="s">
+      <c r="D10" s="86"/>
+      <c r="E10" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="81"/>
+      <c r="F10" s="85"/>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="83"/>
+      <c r="D11" s="87"/>
       <c r="E11" s="28" t="s">
         <v>47</v>
       </c>
@@ -9599,7 +9707,7 @@
       </c>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="83"/>
+      <c r="D12" s="87"/>
       <c r="E12" s="28" t="s">
         <v>48</v>
       </c>
@@ -9609,7 +9717,7 @@
       </c>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="83"/>
+      <c r="D13" s="87"/>
       <c r="E13" s="28" t="s">
         <v>49</v>
       </c>
@@ -9619,7 +9727,7 @@
       </c>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="83"/>
+      <c r="D14" s="87"/>
       <c r="E14" s="28" t="s">
         <v>41</v>
       </c>
@@ -9629,7 +9737,7 @@
       </c>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="83"/>
+      <c r="D15" s="87"/>
       <c r="E15" s="28" t="s">
         <v>50</v>
       </c>
@@ -9639,7 +9747,7 @@
       </c>
     </row>
     <row r="16" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="83"/>
+      <c r="D16" s="87"/>
       <c r="E16" s="28" t="s">
         <v>51</v>
       </c>
@@ -9649,7 +9757,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="83"/>
+      <c r="D17" s="87"/>
       <c r="E17" s="28" t="s">
         <v>52</v>
       </c>
@@ -9659,7 +9767,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="83"/>
+      <c r="D18" s="87"/>
       <c r="E18" s="28" t="s">
         <v>53</v>
       </c>
@@ -9669,7 +9777,7 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="83"/>
+      <c r="D19" s="87"/>
       <c r="E19" s="28" t="s">
         <v>54</v>
       </c>
@@ -9679,7 +9787,7 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="83"/>
+      <c r="D20" s="87"/>
       <c r="E20" s="28" t="s">
         <v>55</v>
       </c>
@@ -9689,7 +9797,7 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="83"/>
+      <c r="D21" s="87"/>
       <c r="E21" s="28" t="s">
         <v>56</v>
       </c>
@@ -9699,14 +9807,14 @@
       </c>
     </row>
     <row r="22" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D22" s="83"/>
+      <c r="D22" s="87"/>
       <c r="E22" s="32" t="s">
         <v>57</v>
       </c>
       <c r="F22" s="31"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="83"/>
+      <c r="D23" s="87"/>
       <c r="E23" s="28" t="s">
         <v>58</v>
       </c>
@@ -9716,7 +9824,7 @@
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="83"/>
+      <c r="D24" s="87"/>
       <c r="E24" s="28" t="s">
         <v>59</v>
       </c>
@@ -9726,14 +9834,14 @@
       </c>
     </row>
     <row r="25" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D25" s="83"/>
+      <c r="D25" s="87"/>
       <c r="E25" s="32" t="s">
         <v>60</v>
       </c>
       <c r="F25" s="31"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="83"/>
+      <c r="D26" s="87"/>
       <c r="E26" s="27" t="s">
         <v>62</v>
       </c>
@@ -9743,7 +9851,7 @@
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="84"/>
+      <c r="D27" s="88"/>
       <c r="E27" s="27" t="s">
         <v>63</v>
       </c>
@@ -9756,13 +9864,13 @@
       <c r="D28" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="76" t="s">
+      <c r="E28" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="77"/>
+      <c r="F28" s="81"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="85"/>
+      <c r="D29" s="89"/>
       <c r="E29" s="27" t="s">
         <v>41</v>
       </c>
@@ -9772,7 +9880,7 @@
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="86"/>
+      <c r="D30" s="90"/>
       <c r="E30" s="27" t="s">
         <v>42</v>
       </c>
@@ -9782,7 +9890,7 @@
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="86"/>
+      <c r="D31" s="90"/>
       <c r="E31" s="27" t="s">
         <v>43</v>
       </c>
@@ -9792,7 +9900,7 @@
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="86"/>
+      <c r="D32" s="90"/>
       <c r="E32" s="27" t="s">
         <v>44</v>
       </c>
@@ -9802,7 +9910,7 @@
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="87"/>
+      <c r="D33" s="91"/>
       <c r="E33" s="27" t="s">
         <v>45</v>
       </c>
@@ -9815,13 +9923,13 @@
       <c r="D34" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="76" t="s">
+      <c r="E34" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="77"/>
+      <c r="F34" s="81"/>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D35" s="85"/>
+      <c r="D35" s="89"/>
       <c r="E35" s="27" t="s">
         <v>67</v>
       </c>
@@ -9831,7 +9939,7 @@
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="86"/>
+      <c r="D36" s="90"/>
       <c r="E36" s="27" t="s">
         <v>68</v>
       </c>
@@ -9841,7 +9949,7 @@
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="86"/>
+      <c r="D37" s="90"/>
       <c r="E37" s="27" t="s">
         <v>69</v>
       </c>
@@ -9851,7 +9959,7 @@
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="86"/>
+      <c r="D38" s="90"/>
       <c r="E38" s="27" t="s">
         <v>70</v>
       </c>
@@ -9861,7 +9969,7 @@
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D39" s="87"/>
+      <c r="D39" s="91"/>
       <c r="E39" s="27" t="s">
         <v>71</v>
       </c>
@@ -9874,13 +9982,13 @@
       <c r="D40" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E40" s="76" t="s">
+      <c r="E40" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="F40" s="77"/>
+      <c r="F40" s="81"/>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D41" s="85"/>
+      <c r="D41" s="89"/>
       <c r="E41" s="27" t="s">
         <v>73</v>
       </c>
@@ -9890,7 +9998,7 @@
       </c>
     </row>
     <row r="42" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D42" s="86"/>
+      <c r="D42" s="90"/>
       <c r="E42" s="27" t="s">
         <v>74</v>
       </c>
@@ -9900,7 +10008,7 @@
       </c>
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D43" s="87"/>
+      <c r="D43" s="91"/>
       <c r="E43" s="27" t="s">
         <v>75</v>
       </c>
@@ -9913,20 +10021,20 @@
       <c r="D44" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="76" t="s">
+      <c r="E44" s="80" t="s">
         <v>133</v>
       </c>
-      <c r="F44" s="77"/>
+      <c r="F44" s="81"/>
     </row>
     <row r="45" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D45" s="85"/>
-      <c r="E45" s="78" t="s">
+      <c r="D45" s="89"/>
+      <c r="E45" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="F45" s="79"/>
+      <c r="F45" s="83"/>
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D46" s="86"/>
+      <c r="D46" s="90"/>
       <c r="E46" s="27" t="s">
         <v>78</v>
       </c>
@@ -9936,7 +10044,7 @@
       </c>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="86"/>
+      <c r="D47" s="90"/>
       <c r="E47" s="27" t="s">
         <v>79</v>
       </c>
@@ -9946,7 +10054,7 @@
       </c>
     </row>
     <row r="48" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D48" s="86"/>
+      <c r="D48" s="90"/>
       <c r="E48" s="27" t="s">
         <v>80</v>
       </c>
@@ -9956,7 +10064,7 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="86"/>
+      <c r="D49" s="90"/>
       <c r="E49" s="27" t="s">
         <v>81</v>
       </c>
@@ -9966,7 +10074,7 @@
       </c>
     </row>
     <row r="50" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D50" s="86"/>
+      <c r="D50" s="90"/>
       <c r="E50" s="27" t="s">
         <v>82</v>
       </c>
@@ -9976,7 +10084,7 @@
       </c>
     </row>
     <row r="51" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D51" s="86"/>
+      <c r="D51" s="90"/>
       <c r="E51" s="27" t="s">
         <v>83</v>
       </c>
@@ -9986,14 +10094,14 @@
       </c>
     </row>
     <row r="52" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D52" s="86"/>
-      <c r="E52" s="78" t="s">
+      <c r="D52" s="90"/>
+      <c r="E52" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="F52" s="79"/>
+      <c r="F52" s="83"/>
     </row>
     <row r="53" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D53" s="86"/>
+      <c r="D53" s="90"/>
       <c r="E53" s="27" t="s">
         <v>86</v>
       </c>
@@ -10003,14 +10111,14 @@
       </c>
     </row>
     <row r="54" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D54" s="86"/>
-      <c r="E54" s="78" t="s">
+      <c r="D54" s="90"/>
+      <c r="E54" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="F54" s="79"/>
+      <c r="F54" s="83"/>
     </row>
     <row r="55" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D55" s="86"/>
+      <c r="D55" s="90"/>
       <c r="E55" s="27" t="s">
         <v>87</v>
       </c>
@@ -10020,7 +10128,7 @@
       </c>
     </row>
     <row r="56" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D56" s="86"/>
+      <c r="D56" s="90"/>
       <c r="E56" s="27" t="s">
         <v>89</v>
       </c>
@@ -10030,7 +10138,7 @@
       </c>
     </row>
     <row r="57" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D57" s="87"/>
+      <c r="D57" s="91"/>
       <c r="E57" s="27" t="s">
         <v>90</v>
       </c>
@@ -10043,17 +10151,17 @@
       <c r="D58" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="E58" s="76" t="s">
+      <c r="E58" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="F58" s="77"/>
+      <c r="F58" s="81"/>
     </row>
     <row r="59" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D59" s="27"/>
-      <c r="E59" s="78" t="s">
+      <c r="E59" s="82" t="s">
         <v>93</v>
       </c>
-      <c r="F59" s="79"/>
+      <c r="F59" s="83"/>
     </row>
     <row r="60" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D60" s="27"/>
@@ -10097,10 +10205,10 @@
     </row>
     <row r="64" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D64" s="27"/>
-      <c r="E64" s="78" t="s">
+      <c r="E64" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="F64" s="79"/>
+      <c r="F64" s="83"/>
     </row>
     <row r="65" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D65" s="27"/>
@@ -10124,10 +10232,10 @@
     </row>
     <row r="67" spans="4:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D67" s="27"/>
-      <c r="E67" s="78" t="s">
+      <c r="E67" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="F67" s="79"/>
+      <c r="F67" s="83"/>
     </row>
     <row r="68" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D68" s="27"/>
@@ -10163,10 +10271,10 @@
       <c r="D71" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="E71" s="76" t="s">
+      <c r="E71" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="F71" s="77"/>
+      <c r="F71" s="81"/>
     </row>
     <row r="72" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D72" s="27"/>
@@ -10182,10 +10290,10 @@
       <c r="D73" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E73" s="76" t="s">
+      <c r="E73" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="F73" s="77"/>
+      <c r="F73" s="81"/>
     </row>
     <row r="74" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D74" s="27"/>
@@ -10221,10 +10329,10 @@
       <c r="D77" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="E77" s="76" t="s">
+      <c r="E77" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="F77" s="77"/>
+      <c r="F77" s="81"/>
     </row>
     <row r="78" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D78" s="27"/>
@@ -11779,7 +11887,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="C1:AW28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
@@ -11799,210 +11907,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:49" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="89"/>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
-      <c r="AF1" s="89"/>
-      <c r="AG1" s="89"/>
-      <c r="AH1" s="89"/>
-      <c r="AI1" s="89"/>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="89"/>
-      <c r="AL1" s="89"/>
-      <c r="AM1" s="89"/>
-      <c r="AN1" s="89"/>
-      <c r="AO1" s="89"/>
-      <c r="AP1" s="89"/>
-      <c r="AQ1" s="89"/>
-      <c r="AR1" s="89"/>
-      <c r="AS1" s="89"/>
-      <c r="AT1" s="89"/>
-      <c r="AU1" s="89"/>
-      <c r="AV1" s="89"/>
-      <c r="AW1" s="89"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
+      <c r="R1" s="93"/>
+      <c r="S1" s="93"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="93"/>
+      <c r="V1" s="93"/>
+      <c r="W1" s="93"/>
+      <c r="X1" s="93"/>
+      <c r="Y1" s="93"/>
+      <c r="Z1" s="93"/>
+      <c r="AA1" s="93"/>
+      <c r="AB1" s="93"/>
+      <c r="AC1" s="93"/>
+      <c r="AD1" s="93"/>
+      <c r="AE1" s="93"/>
+      <c r="AF1" s="93"/>
+      <c r="AG1" s="93"/>
+      <c r="AH1" s="93"/>
+      <c r="AI1" s="93"/>
+      <c r="AJ1" s="93"/>
+      <c r="AK1" s="93"/>
+      <c r="AL1" s="93"/>
+      <c r="AM1" s="93"/>
+      <c r="AN1" s="93"/>
+      <c r="AO1" s="93"/>
+      <c r="AP1" s="93"/>
+      <c r="AQ1" s="93"/>
+      <c r="AR1" s="93"/>
+      <c r="AS1" s="93"/>
+      <c r="AT1" s="93"/>
+      <c r="AU1" s="93"/>
+      <c r="AV1" s="93"/>
+      <c r="AW1" s="93"/>
     </row>
     <row r="2" spans="3:49" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="89"/>
-      <c r="AA2" s="89"/>
-      <c r="AB2" s="89"/>
-      <c r="AC2" s="89"/>
-      <c r="AD2" s="89"/>
-      <c r="AE2" s="89"/>
-      <c r="AF2" s="89"/>
-      <c r="AG2" s="89"/>
-      <c r="AH2" s="89"/>
-      <c r="AI2" s="89"/>
-      <c r="AJ2" s="89"/>
-      <c r="AK2" s="89"/>
-      <c r="AL2" s="89"/>
-      <c r="AM2" s="89"/>
-      <c r="AN2" s="89"/>
-      <c r="AO2" s="89"/>
-      <c r="AP2" s="89"/>
-      <c r="AQ2" s="89"/>
-      <c r="AR2" s="89"/>
-      <c r="AS2" s="89"/>
-      <c r="AT2" s="89"/>
-      <c r="AU2" s="89"/>
-      <c r="AV2" s="89"/>
-      <c r="AW2" s="89"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="93"/>
+      <c r="Y2" s="93"/>
+      <c r="Z2" s="93"/>
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="93"/>
+      <c r="AG2" s="93"/>
+      <c r="AH2" s="93"/>
+      <c r="AI2" s="93"/>
+      <c r="AJ2" s="93"/>
+      <c r="AK2" s="93"/>
+      <c r="AL2" s="93"/>
+      <c r="AM2" s="93"/>
+      <c r="AN2" s="93"/>
+      <c r="AO2" s="93"/>
+      <c r="AP2" s="93"/>
+      <c r="AQ2" s="93"/>
+      <c r="AR2" s="93"/>
+      <c r="AS2" s="93"/>
+      <c r="AT2" s="93"/>
+      <c r="AU2" s="93"/>
+      <c r="AV2" s="93"/>
+      <c r="AW2" s="93"/>
     </row>
     <row r="3" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="63"/>
-      <c r="AD3" s="63"/>
-      <c r="AE3" s="63"/>
-      <c r="AF3" s="63"/>
-      <c r="AG3" s="63"/>
-      <c r="AH3" s="63"/>
-      <c r="AI3" s="63"/>
-      <c r="AJ3" s="63"/>
-      <c r="AK3" s="63"/>
-      <c r="AL3" s="63"/>
-      <c r="AM3" s="63"/>
-      <c r="AN3" s="63"/>
-      <c r="AO3" s="63"/>
-      <c r="AP3" s="63"/>
-      <c r="AQ3" s="63"/>
-      <c r="AR3" s="63"/>
-      <c r="AS3" s="63"/>
-      <c r="AT3" s="63"/>
-      <c r="AU3" s="63"/>
-      <c r="AV3" s="63"/>
-      <c r="AW3" s="64"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
+      <c r="AJ3" s="67"/>
+      <c r="AK3" s="67"/>
+      <c r="AL3" s="67"/>
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
+      <c r="AV3" s="67"/>
+      <c r="AW3" s="68"/>
     </row>
     <row r="4" spans="3:49" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="66"/>
-      <c r="W4" s="66"/>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="66"/>
-      <c r="AG4" s="66"/>
-      <c r="AH4" s="66"/>
-      <c r="AI4" s="66"/>
-      <c r="AJ4" s="66"/>
-      <c r="AK4" s="66"/>
-      <c r="AL4" s="66"/>
-      <c r="AM4" s="66"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="66"/>
-      <c r="AQ4" s="66"/>
-      <c r="AR4" s="66"/>
-      <c r="AS4" s="66"/>
-      <c r="AT4" s="66"/>
-      <c r="AU4" s="66"/>
-      <c r="AV4" s="66"/>
-      <c r="AW4" s="67"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="70"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="70"/>
+      <c r="AD4" s="70"/>
+      <c r="AE4" s="70"/>
+      <c r="AF4" s="70"/>
+      <c r="AG4" s="70"/>
+      <c r="AH4" s="70"/>
+      <c r="AI4" s="70"/>
+      <c r="AJ4" s="70"/>
+      <c r="AK4" s="70"/>
+      <c r="AL4" s="70"/>
+      <c r="AM4" s="70"/>
+      <c r="AN4" s="70"/>
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="70"/>
+      <c r="AQ4" s="70"/>
+      <c r="AR4" s="70"/>
+      <c r="AS4" s="70"/>
+      <c r="AT4" s="70"/>
+      <c r="AU4" s="70"/>
+      <c r="AV4" s="70"/>
+      <c r="AW4" s="71"/>
     </row>
     <row r="5" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="92"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="96"/>
       <c r="G5" s="17">
         <f ca="1">TODAY()</f>
         <v>44700</v>
@@ -12055,12 +12163,12 @@
       <c r="AW5" s="9"/>
     </row>
     <row r="6" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C6" s="93" t="s">
+      <c r="C6" s="97" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="95"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="99"/>
       <c r="G6" s="4" t="s">
         <v>130</v>
       </c>
@@ -12078,22 +12186,22 @@
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
-      <c r="V6" s="75" t="s">
+      <c r="V6" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="75"/>
-      <c r="X6" s="74">
+      <c r="W6" s="79"/>
+      <c r="X6" s="78">
         <v>2022</v>
       </c>
-      <c r="Y6" s="74"/>
-      <c r="Z6" s="74"/>
+      <c r="Y6" s="78"/>
+      <c r="Z6" s="78"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
-      <c r="AC6" s="75" t="s">
+      <c r="AC6" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="AD6" s="75"/>
-      <c r="AE6" s="75"/>
+      <c r="AD6" s="79"/>
+      <c r="AE6" s="79"/>
       <c r="AF6" s="18">
         <v>5</v>
       </c>
@@ -12165,31 +12273,31 @@
       <c r="AW7" s="9"/>
     </row>
     <row r="8" spans="3:49" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="96" t="s">
+      <c r="C8" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="88" t="s">
+      <c r="D8" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="88" t="s">
+      <c r="E8" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="88" t="s">
+      <c r="G8" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="88" t="s">
+      <c r="H8" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="88" t="s">
+      <c r="I8" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="88" t="s">
+      <c r="J8" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="88" t="s">
+      <c r="K8" s="92" t="s">
         <v>17</v>
       </c>
       <c r="L8" s="41" t="s">
@@ -12308,15 +12416,15 @@
       </c>
     </row>
     <row r="9" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C9" s="96"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
       <c r="L9" s="44">
         <f>DATE($X$6,$AF$6,1)-WEEKDAY(DATE($X$6,$AF$6,1),1)+1</f>
         <v>44682</v>
@@ -12471,7 +12579,7 @@
       </c>
     </row>
     <row r="10" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C10" s="97" t="s">
+      <c r="C10" s="101" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="46" t="s">
@@ -12480,7 +12588,7 @@
       <c r="E10" s="47">
         <v>28</v>
       </c>
-      <c r="F10" s="99">
+      <c r="F10" s="103">
         <v>2</v>
       </c>
       <c r="G10" s="48">
@@ -12534,14 +12642,14 @@
       <c r="AW10" s="19"/>
     </row>
     <row r="11" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C11" s="98"/>
+      <c r="C11" s="102"/>
       <c r="D11" s="46" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="47">
         <v>18</v>
       </c>
-      <c r="F11" s="100"/>
+      <c r="F11" s="104"/>
       <c r="G11" s="48">
         <v>44698</v>
       </c>
@@ -12593,15 +12701,15 @@
       <c r="AW11" s="19"/>
     </row>
     <row r="12" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="101"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="102"/>
-      <c r="J12" s="102"/>
-      <c r="K12" s="103"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="106"/>
+      <c r="H12" s="106"/>
+      <c r="I12" s="106"/>
+      <c r="J12" s="106"/>
+      <c r="K12" s="107"/>
       <c r="L12" s="39"/>
       <c r="M12" s="39"/>
       <c r="N12" s="39"/>
@@ -12642,7 +12750,7 @@
       <c r="AW12" s="19"/>
     </row>
     <row r="13" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C13" s="97" t="s">
+      <c r="C13" s="101" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="46" t="s">
@@ -12651,7 +12759,7 @@
       <c r="E13" s="47">
         <v>24</v>
       </c>
-      <c r="F13" s="99">
+      <c r="F13" s="103">
         <v>2</v>
       </c>
       <c r="G13" s="48">
@@ -12705,14 +12813,14 @@
       <c r="AW13" s="19"/>
     </row>
     <row r="14" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C14" s="98"/>
+      <c r="C14" s="102"/>
       <c r="D14" s="46" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="47">
         <v>17</v>
       </c>
-      <c r="F14" s="100"/>
+      <c r="F14" s="104"/>
       <c r="G14" s="48">
         <v>44698</v>
       </c>
@@ -12764,15 +12872,15 @@
       <c r="AW14" s="19"/>
     </row>
     <row r="15" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="102"/>
-      <c r="I15" s="102"/>
-      <c r="J15" s="102"/>
-      <c r="K15" s="103"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="106"/>
+      <c r="I15" s="106"/>
+      <c r="J15" s="106"/>
+      <c r="K15" s="107"/>
       <c r="L15" s="39"/>
       <c r="M15" s="39"/>
       <c r="N15" s="39"/>
@@ -12813,7 +12921,7 @@
       <c r="AW15" s="19"/>
     </row>
     <row r="16" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C16" s="97" t="s">
+      <c r="C16" s="101" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="46" t="s">
@@ -12822,7 +12930,7 @@
       <c r="E16" s="47">
         <v>19</v>
       </c>
-      <c r="F16" s="99">
+      <c r="F16" s="103">
         <v>1</v>
       </c>
       <c r="G16" s="48">
@@ -12876,14 +12984,14 @@
       <c r="AW16" s="19"/>
     </row>
     <row r="17" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C17" s="98"/>
+      <c r="C17" s="102"/>
       <c r="D17" s="46" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="47">
         <v>17</v>
       </c>
-      <c r="F17" s="100"/>
+      <c r="F17" s="104"/>
       <c r="G17" s="48">
         <v>44698</v>
       </c>
@@ -12935,15 +13043,15 @@
       <c r="AW17" s="19"/>
     </row>
     <row r="18" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="102"/>
-      <c r="I18" s="102"/>
-      <c r="J18" s="102"/>
-      <c r="K18" s="103"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106"/>
+      <c r="K18" s="107"/>
       <c r="L18" s="39"/>
       <c r="M18" s="39"/>
       <c r="N18" s="39"/>
@@ -12984,7 +13092,7 @@
       <c r="AW18" s="19"/>
     </row>
     <row r="19" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C19" s="97" t="s">
+      <c r="C19" s="101" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="46" t="s">
@@ -12993,7 +13101,7 @@
       <c r="E19" s="47">
         <v>22</v>
       </c>
-      <c r="F19" s="99">
+      <c r="F19" s="103">
         <v>1</v>
       </c>
       <c r="G19" s="48">
@@ -13047,14 +13155,14 @@
       <c r="AW19" s="19"/>
     </row>
     <row r="20" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C20" s="98"/>
+      <c r="C20" s="102"/>
       <c r="D20" s="46" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="47">
         <v>17</v>
       </c>
-      <c r="F20" s="100"/>
+      <c r="F20" s="104"/>
       <c r="G20" s="48">
         <v>44698</v>
       </c>
@@ -13155,7 +13263,7 @@
       <c r="AW21" s="19"/>
     </row>
     <row r="22" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C22" s="97" t="s">
+      <c r="C22" s="101" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="46" t="s">
@@ -13164,7 +13272,7 @@
       <c r="E22" s="47">
         <v>0</v>
       </c>
-      <c r="F22" s="99">
+      <c r="F22" s="103">
         <v>0</v>
       </c>
       <c r="G22" s="48"/>
@@ -13214,14 +13322,14 @@
       <c r="AW22" s="19"/>
     </row>
     <row r="23" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C23" s="98"/>
+      <c r="C23" s="102"/>
       <c r="D23" s="46" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="47">
         <v>0</v>
       </c>
-      <c r="F23" s="100"/>
+      <c r="F23" s="104"/>
       <c r="G23" s="48"/>
       <c r="H23" s="48"/>
       <c r="I23" s="48"/>
@@ -13269,15 +13377,15 @@
       <c r="AW23" s="19"/>
     </row>
     <row r="24" spans="3:49" ht="4.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="101"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="102"/>
-      <c r="I24" s="102"/>
-      <c r="J24" s="102"/>
-      <c r="K24" s="103"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="106"/>
+      <c r="F24" s="106"/>
+      <c r="G24" s="106"/>
+      <c r="H24" s="106"/>
+      <c r="I24" s="106"/>
+      <c r="J24" s="106"/>
+      <c r="K24" s="107"/>
       <c r="L24" s="39"/>
       <c r="M24" s="39"/>
       <c r="N24" s="39"/>
@@ -13318,7 +13426,7 @@
       <c r="AW24" s="19"/>
     </row>
     <row r="25" spans="3:49" x14ac:dyDescent="0.25">
-      <c r="C25" s="97" t="s">
+      <c r="C25" s="101" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="46" t="s">
@@ -13327,7 +13435,7 @@
       <c r="E25" s="47">
         <v>11</v>
       </c>
-      <c r="F25" s="99">
+      <c r="F25" s="103">
         <v>1</v>
       </c>
       <c r="G25" s="48">
@@ -13381,14 +13489,14 @@
       <c r="AW25" s="19"/>
     </row>
     <row r="26" spans="3:49" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="104"/>
+      <c r="C26" s="108"/>
       <c r="D26" s="56" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="57">
         <v>11</v>
       </c>
-      <c r="F26" s="105"/>
+      <c r="F26" s="109"/>
       <c r="G26" s="58">
         <v>44698</v>
       </c>
@@ -13489,10 +13597,10 @@
     <mergeCell ref="G8:G9"/>
   </mergeCells>
   <conditionalFormatting sqref="L9:AW9">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>AND(YEAR(TODAY())=$X$6,MONTH(TODAY())=$AF$6,DAY(L9)=DAY(TODAY()),MONTH(L9)=$AF$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>MONTH(L9)&lt;&gt;$AF$6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13511,31 +13619,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:AW26">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="24" priority="6">
       <formula>AND(L$9&gt;=$I10,L$9&lt;=$J10)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>L$9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>AND(L$9&gt;=$G10,L$9&lt;=$H10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>M$9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="20" priority="10">
       <formula>AND(M$9&gt;=$G6,M$9&lt;=$H6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6:Z6">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>YEAR(TODAY())=$X$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF6">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>AND(YEAR(TODAY())=$X$6,MONTH(TODAY())=$AF$6)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>